<commit_message>
Task 3.8 (Global fixes & plotting multiple diagrams on single sheet)
</commit_message>
<xml_diff>
--- a/olympiad_analysis/norway_beatlon.xlsx
+++ b/olympiad_analysis/norway_beatlon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rexandel\Desktop\GitHub\big_data_research\olympiad_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DDDE35-273F-4E33-AF80-2FBFA63A82AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72E49E5-0609-45F7-A747-497B426EEF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CF086F1-F5FC-4AD6-8255-4DF0CBD20F6A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Olympiad</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Albertville (1992)</t>
-  </si>
-  <si>
-    <t>Top three</t>
   </si>
 </sst>
 </file>
@@ -563,7 +560,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,9 +601,7 @@
       <c r="I1" s="9">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="J1" s="13"/>
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
       <c r="M1" s="13"/>
@@ -645,10 +640,7 @@
       <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="5">
-        <f>SUM(B2:D2)</f>
-        <v>0</v>
-      </c>
+      <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -685,10 +677,7 @@
       <c r="I3" s="5">
         <v>0</v>
       </c>
-      <c r="J3" s="5">
-        <f t="shared" ref="J3:J10" si="0">SUM(B3:D3)</f>
-        <v>0</v>
-      </c>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -725,10 +714,7 @@
       <c r="I4" s="5">
         <v>2</v>
       </c>
-      <c r="J4" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="J4" s="4"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -765,10 +751,7 @@
       <c r="I5" s="5">
         <v>2</v>
       </c>
-      <c r="J5" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -805,10 +788,7 @@
       <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -845,10 +825,7 @@
       <c r="I7" s="5">
         <v>2</v>
       </c>
-      <c r="J7" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="J7" s="4"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -885,10 +862,7 @@
       <c r="I8" s="5">
         <v>1</v>
       </c>
-      <c r="J8" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="J8" s="4"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -925,10 +899,7 @@
       <c r="I9" s="5">
         <v>2</v>
       </c>
-      <c r="J9" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="J9" s="4"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -965,10 +936,7 @@
       <c r="I10" s="7">
         <v>1</v>
       </c>
-      <c r="J10" s="7">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
+      <c r="J10" s="4"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>

</xml_diff>